<commit_message>
commit final - alterações após reunião interna
</commit_message>
<xml_diff>
--- a/DADOS/parcerias_lat_long.xlsx
+++ b/DADOS/parcerias_lat_long.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://spparceriassa-my.sharepoint.com/personal/vitorio_aflalo_spparcerias_com_br/Documents/Área de Trabalho/PROJETOS/DASHBOARDS SOCIAIS/INDICADORES BASE/MAPA-SHINY/DADOS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="351" documentId="11_5C3D73BED3F05465B3F93711595ED87656CFE358" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5C1164F1-B08C-48F4-BE5A-A8D195118CF0}"/>
+  <xr:revisionPtr revIDLastSave="353" documentId="11_5C3D73BED3F05465B3F93711595ED87656CFE358" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CE13A6D-6F19-4A0F-AF19-62F43AA4BA6B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,9 +106,6 @@
     <t>Cemitério da Lapa</t>
   </si>
   <si>
-    <t>Cemitério do Lageado</t>
-  </si>
-  <si>
     <t>Crematório da Vila Alpina</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
     <t>Mercado Paulistano</t>
   </si>
   <si>
-    <t>Parque do Lageado</t>
-  </si>
-  <si>
     <t>Parque Brigadeiro Faria Lima</t>
   </si>
   <si>
@@ -701,6 +695,12 @@
   </si>
   <si>
     <t>Termo de permissão de uso (TPU)</t>
+  </si>
+  <si>
+    <t>Cemitério do Lajeado</t>
+  </si>
+  <si>
+    <t>Parque do Lajeado</t>
   </si>
 </sst>
 </file>
@@ -1121,8 +1121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1138,39 +1138,39 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>219</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
@@ -1181,13 +1181,13 @@
         <v>17</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
@@ -1198,13 +1198,13 @@
         <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -1212,47 +1212,47 @@
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
@@ -1261,13 +1261,13 @@
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
@@ -1279,10 +1279,10 @@
         <v>26</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -1291,13 +1291,13 @@
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -1309,10 +1309,10 @@
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -1324,10 +1324,10 @@
         <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -1339,10 +1339,10 @@
         <v>7</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -1351,13 +1351,13 @@
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -1369,10 +1369,10 @@
         <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -1381,13 +1381,13 @@
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -1399,10 +1399,10 @@
         <v>22</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1414,10 +1414,10 @@
         <v>21</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -1429,10 +1429,10 @@
         <v>2</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
@@ -1441,13 +1441,13 @@
     </row>
     <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -1456,13 +1456,13 @@
     </row>
     <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6" t="s">
-        <v>27</v>
+        <v>224</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
@@ -1474,10 +1474,10 @@
         <v>24</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
@@ -1486,13 +1486,13 @@
     </row>
     <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -1504,10 +1504,10 @@
         <v>1</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -1516,13 +1516,13 @@
     </row>
     <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
@@ -1534,10 +1534,10 @@
         <v>19</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
@@ -1546,13 +1546,13 @@
     </row>
     <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
@@ -1561,13 +1561,13 @@
     </row>
     <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -1576,64 +1576,64 @@
     </row>
     <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G29" s="4"/>
     </row>
     <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -1642,54 +1642,54 @@
     </row>
     <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -1697,16 +1697,16 @@
     </row>
     <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -1714,35 +1714,35 @@
     </row>
     <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G37" s="4"/>
     </row>
     <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
@@ -1750,35 +1750,35 @@
     </row>
     <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E39" s="4"/>
       <c r="F39" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G39" s="4"/>
     </row>
     <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
@@ -1786,16 +1786,16 @@
     </row>
     <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
@@ -1803,184 +1803,184 @@
     </row>
     <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G42" s="4"/>
     </row>
     <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G43" s="4"/>
     </row>
     <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G44" s="4"/>
     </row>
     <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E45" s="4"/>
       <c r="F45" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G45" s="4"/>
     </row>
     <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E46" s="4"/>
       <c r="F46" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G46" s="4"/>
     </row>
     <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E47" s="4"/>
       <c r="F47" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G47" s="4"/>
     </row>
     <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E48" s="4"/>
       <c r="F48" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G48" s="4"/>
     </row>
     <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E49" s="4"/>
       <c r="F49" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G49" s="4"/>
     </row>
     <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F50" s="4"/>
       <c r="G50" s="4"/>
     </row>
     <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -1989,13 +1989,13 @@
     </row>
     <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -2007,13 +2007,13 @@
         <v>14</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
@@ -2021,16 +2021,16 @@
     </row>
     <row r="54" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
@@ -2038,16 +2038,16 @@
     </row>
     <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
@@ -2055,16 +2055,16 @@
     </row>
     <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E56" s="4"/>
       <c r="F56" s="4"/>
@@ -2072,16 +2072,16 @@
     </row>
     <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E57" s="4"/>
       <c r="F57" s="4"/>
@@ -2092,13 +2092,13 @@
         <v>6</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E58" s="4"/>
       <c r="F58" s="4"/>
@@ -2106,16 +2106,16 @@
     </row>
     <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6" t="s">
-        <v>35</v>
+        <v>225</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
@@ -2123,16 +2123,16 @@
     </row>
     <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
@@ -2140,16 +2140,16 @@
     </row>
     <row r="61" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
@@ -2157,16 +2157,16 @@
     </row>
     <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
@@ -2177,13 +2177,13 @@
         <v>10</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
@@ -2194,13 +2194,13 @@
         <v>8</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
@@ -2211,13 +2211,13 @@
         <v>9</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
@@ -2228,10 +2228,10 @@
         <v>12</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
@@ -2240,13 +2240,13 @@
     </row>
     <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
@@ -2255,35 +2255,35 @@
     </row>
     <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
       <c r="F68" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G68" s="4"/>
     </row>
     <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
       <c r="F69" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G69" s="4"/>
     </row>
@@ -2292,10 +2292,10 @@
         <v>15</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
@@ -2304,13 +2304,13 @@
     </row>
     <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
@@ -2319,13 +2319,13 @@
     </row>
     <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
@@ -2337,10 +2337,10 @@
         <v>23</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
@@ -2349,13 +2349,13 @@
     </row>
     <row r="74" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
@@ -2364,30 +2364,30 @@
     </row>
     <row r="75" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
       <c r="F75" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G75" s="4"/>
     </row>
     <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -2396,13 +2396,13 @@
     </row>
     <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
@@ -2411,64 +2411,64 @@
     </row>
     <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
       <c r="F78" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G78" s="4"/>
     </row>
     <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
       <c r="F79" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G79" s="4"/>
     </row>
     <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D80" s="4"/>
       <c r="E80" s="4"/>
       <c r="F80" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G80" s="4"/>
     </row>
     <row r="81" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
@@ -2477,13 +2477,13 @@
     </row>
     <row r="82" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
@@ -2492,13 +2492,13 @@
     </row>
     <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
@@ -2510,10 +2510,10 @@
         <v>3</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
@@ -2522,64 +2522,64 @@
     </row>
     <row r="85" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
       <c r="F85" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G85" s="4"/>
     </row>
     <row r="86" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
       <c r="F86" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G86" s="4"/>
     </row>
     <row r="87" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
       <c r="F87" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G87" s="4"/>
     </row>
     <row r="88" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
@@ -2588,35 +2588,35 @@
     </row>
     <row r="89" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
       <c r="F89" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G89" s="4"/>
     </row>
     <row r="90" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
       <c r="F90" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G90" s="4"/>
     </row>
@@ -2625,10 +2625,10 @@
         <v>4</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
@@ -2640,10 +2640,10 @@
         <v>5</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
@@ -2655,10 +2655,10 @@
         <v>11</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
@@ -2667,30 +2667,30 @@
     </row>
     <row r="94" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
       <c r="F94" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G94" s="4"/>
     </row>
     <row r="95" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
@@ -2699,47 +2699,47 @@
     </row>
     <row r="96" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
       <c r="F96" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G96" s="4"/>
     </row>
     <row r="97" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
       <c r="F97" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G97" s="4"/>
     </row>
     <row r="98" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
@@ -2748,37 +2748,37 @@
     </row>
     <row r="99" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
       <c r="F99" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G99" s="4"/>
     </row>
     <row r="100" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E100" s="4"/>
       <c r="F100" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G100" s="4"/>
     </row>
@@ -2787,10 +2787,10 @@
         <v>13</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="4"/>

</xml_diff>